<commit_message>
made changes, added new functions => group df by time interval, and convert df to json
</commit_message>
<xml_diff>
--- a/excel data/FRIDAY.xlsx
+++ b/excel data/FRIDAY.xlsx
@@ -898,7 +898,7 @@
       </c>
       <c r="AV2" t="inlineStr">
         <is>
-          <t>AS</t>
+          <t>RLN</t>
         </is>
       </c>
       <c r="AW2" t="n">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="Y4" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="Q5" t="n">
@@ -1499,7 +1499,7 @@
         </is>
       </c>
       <c r="AC5" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>TC/BJM</t>
+          <t>TAC/BJM</t>
         </is>
       </c>
       <c r="AG5" t="n">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="AK5" t="n">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="AO5" t="n">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AMS/CS/SL</t>
         </is>
       </c>
       <c r="AC6" t="n">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AMS/CS/SL</t>
         </is>
       </c>
       <c r="AG6" t="n">
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MP</t>
         </is>
       </c>
       <c r="Q11" t="n">
@@ -2903,7 +2903,7 @@
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MP</t>
         </is>
       </c>
       <c r="AK11" t="n">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="AN11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MP</t>
         </is>
       </c>
       <c r="AO11" t="n">
@@ -3118,7 +3118,7 @@
         </is>
       </c>
       <c r="Y12" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
@@ -3136,7 +3136,7 @@
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
@@ -3839,7 +3839,7 @@
         </is>
       </c>
       <c r="Y15" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
         </is>
       </c>
       <c r="AC15" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
@@ -4100,7 +4100,7 @@
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="AD16" t="inlineStr">
         <is>
@@ -4343,7 +4343,7 @@
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
@@ -4829,7 +4829,7 @@
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
@@ -5558,7 +5558,7 @@
         </is>
       </c>
       <c r="AC22" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="AD22" t="inlineStr">
         <is>
@@ -5797,11 +5797,11 @@
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>(BS/LP/AS)</t>
+          <t>BS/LP/AS</t>
         </is>
       </c>
       <c r="AC23" t="n">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="AD23" t="inlineStr">
         <is>
@@ -6044,7 +6044,7 @@
         </is>
       </c>
       <c r="AC24" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AD24" t="inlineStr">
         <is>
@@ -6283,7 +6283,7 @@
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>GN/CK</t>
+          <t>FGN/CK</t>
         </is>
       </c>
       <c r="AC25" t="n">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>GN/CK</t>
+          <t>FGN/CK</t>
         </is>
       </c>
       <c r="AG25" t="n">

</xml_diff>